<commit_message>
Up to coins in ruins
</commit_message>
<xml_diff>
--- a/synacor/rpg_maze.xlsx
+++ b/synacor/rpg_maze.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\AoC2019\synacor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD62BE5-730F-4486-B940-551F16063490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C4356D-453C-41DA-A421-738FD9E02975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41460" yWindow="795" windowWidth="21600" windowHeight="11385" xr2:uid="{A4590512-B461-4D61-BB7F-4AF2383C5086}"/>
+    <workbookView xWindow="-28800" yWindow="795" windowWidth="21600" windowHeight="11385" xr2:uid="{A4590512-B461-4D61-BB7F-4AF2383C5086}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>== Foothills ==
 You find yourself standing at the base of an enormous mountain.  At its base to the north, there is a massive doorway.  A sign nearby reads "Keep out!  Definitely no treasure within!"
@@ -86,35 +86,6 @@
 - down                                                                                      </t>
   </si>
   <si>
-    <t>== Moss cavern ==
-You are standing in a large cavern full of bioluminescent moss.  It must have broken your fall!  The cavern extends to the east and west; at the west end, you think you see a passage leading out of the cavern.
-There are 2 exits:
-- west
-- east</t>
-  </si>
-  <si>
-    <t>== Moss cavern ==
-You are standing in a large cavern full of bioluminescent moss.  The cavern extends to the east.  There is a crevise in the rocks which opens into a passage.
-There are 2 exits:
-- east
-- passage</t>
-  </si>
-  <si>
-    <t>== Passage ==
-You are in a crevise on the west wall of the moss cavern.  A dark passage leads further west.  There is a ladder here which leads down into a smaller, moss-filled cavern below.
-There are 3 exits:
-- cavern
-- ladder
-- darkness</t>
-  </si>
-  <si>
-    <t>== Passage ==
-It is pitch black.  You are likely to be eaten by a grue.
-There are 2 exits:
-- continue
-- back</t>
-  </si>
-  <si>
     <t xml:space="preserve">== Fumbling around in the darkness ==                                                       
 Without a source of light, you have become hopelessly lost and are fumbling around in the da
 rkness.                                                                                     
@@ -149,7 +120,121 @@
     <t>Back: DEATH</t>
   </si>
   <si>
-    <t xml:space="preserve">== Twisty passages ==                                                                       
+    <t>== Twisty passages ==
+You are in a maze of little twisty passages, all alike.
+There are 3 exits:
+- north
+- south
+- east</t>
+  </si>
+  <si>
+    <t>== Twisty passages ==
+You are in a twisty maze of little passages, all alike.
+There are 3 exits:
+- north
+- south
+- west</t>
+  </si>
+  <si>
+    <t>== Twisty passages ==
+You are in a maze of twisty little passages, all dimly lit by more bioluminescent moss.  There is a ladder here leading up.
+There are 5 exits:
+- ladder
+- north
+- south
+- east
+- west</t>
+  </si>
+  <si>
+    <t>== Twisty passages ==
+You are in a little maze of twisty passages, all alike.
+There are 3 exits:
+- north
+- south
+- east</t>
+  </si>
+  <si>
+    <t>== Twisty passages ==
+You are in a twisty alike of little passages, all maze.
+The east passage appears very dark; you feel likely to be eaten by a Grue.
+There are 4 exits:
+- north
+- south
+- west
+- east</t>
+  </si>
+  <si>
+    <t>DEATH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+== Twisty passages ==
+You are in a little maze of twisty passages, all alike.
+There are 3 exits:
+- north
+- south
+- east</t>
+  </si>
+  <si>
+    <t>== Twisty passages == 2402
+You are in a maze of alike little passages, all twisty.
+The passage to the east looks very dark; you think you hear a Grue.
+There are 4 exits:
+- north
+- south
+- west
+- east</t>
+  </si>
+  <si>
+    <t>== Twisty passages == 2407
+You are in a maze of alike twisty passages, all little.
+There are 3 exits:
+- north
+- east
+- south</t>
+  </si>
+  <si>
+    <t>2387</t>
+  </si>
+  <si>
+    <t>== Moss cavern == (2352)
+You are standing in a large cavern full of bioluminescent moss.  It must have broken your fall!  The cavern extends to the east and west; at the west end, you think you see a passage leading out of the cavern.
+There are 2 exits:
+- west
+- east</t>
+  </si>
+  <si>
+    <t>== Moss cavern == (2357)
+You are standing in a large cavern full of bioluminescent moss.  The cavern extends to the west.
+Things of interest here:
+- empty lantern
+There is 1 exit:
+- west</t>
+  </si>
+  <si>
+    <t>== Passage == (2367)
+You are in a crevise on the west wall of the moss cavern.  A dark passage leads further west.  There is a ladder here which leads down into a smaller, moss-filled cavern below.
+There are 3 exits:
+- cavern
+- ladder
+- darkness</t>
+  </si>
+  <si>
+    <t>== Passage == (2372)
+It is pitch black.  You are likely to be eaten by a grue.
+There are 2 exits:
+- continue
+- back</t>
+  </si>
+  <si>
+    <t>== Moss cavern == (2362)
+You are standing in a large cavern full of bioluminescent moss.  The cavern extends to the east.  There is a crevise in the rocks which opens into a passage.
+There are 2 exits:
+- east
+- passage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">== Twisty passages ==    (2377)                                                           
 You are in a maze of twisty little passages, all dimly lit by more bioluminescent moss.  The
 re is a ladder here leading up.                                                             
 There are 5 exits:                                                                          
@@ -161,15 +246,7 @@
                                                                                             </t>
   </si>
   <si>
-    <t>== Twisty passages ==
-You are in a maze of little twisty passages, all alike.
-There are 3 exits:
-- north
-- south
-- east</t>
-  </si>
-  <si>
-    <t>== Twisty passages ==
+    <t>== Twisty passages == (2382)
 You are in a twisty maze of little passages, all alike.
 There are 3 exits:
 - north
@@ -177,47 +254,7 @@
 - west</t>
   </si>
   <si>
-    <t>== Twisty passages ==
-You are in a maze of twisty little passages, all dimly lit by more bioluminescent moss.  There is a ladder here leading up.
-There are 5 exits:
-- ladder
-- north
-- south
-- east
-- west</t>
-  </si>
-  <si>
-    <t>== Twisty passages ==
-You are in a little maze of twisty passages, all alike.
-There are 3 exits:
-- north
-- south
-- east</t>
-  </si>
-  <si>
-    <t>== Twisty passages ==
-You are in a twisty alike of little passages, all maze.
-The east passage appears very dark; you feel likely to be eaten by a Grue.
-There are 4 exits:
-- north
-- south
-- west
-- east</t>
-  </si>
-  <si>
-    <t>DEATH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-== Twisty passages ==
-You are in a little maze of twisty passages, all alike.
-There are 3 exits:
-- north
-- south
-- east</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                
+    <t xml:space="preserve">(2417)                                                                                
 Chiseled on the wall of one of the passageways, you see:                        
     xSoSzxDgGMtz                                                                
 You take note of this and keep walking.                                         
@@ -229,25 +266,96 @@
 - west                                                                          </t>
   </si>
   <si>
-    <t>== Twisty passages == 2402
-You are in a maze of alike little passages, all twisty.
-The passage to the east looks very dark; you think you hear a Grue.
-There are 4 exits:
-- north
-- south
+    <t>== Dark passage == (2472)
+You are in a narrow passage.  There is darkness to the west, but you can barely see a glowing opening to the east.
+There are 2 exits:
 - west
 - east</t>
   </si>
   <si>
-    <t>== Twisty passages == 2407
-You are in a maze of alike twisty passages, all little.
-There are 3 exits:
-- north
+    <t>== Dark passage == (2432)
+You are in a dark, narrow passage.
+There are 2 exits:
 - east
+- west</t>
+  </si>
+  <si>
+    <t>== Dark passage == (2437)
+You are in a dark, narrow passage.
+There are 2 exits:
+- east
+- west</t>
+  </si>
+  <si>
+    <t>== Dark passage == (2442)
+You are in a dark, narrow passage.  To the west, you spot some vegetation where the passage expands.
+There are 2 exits:
+- east
+- west</t>
+  </si>
+  <si>
+    <t xml:space="preserve">== Ruins ==      (2447)                                                                 
+You stand in a large cavern with a huge ruin to the north, overgrown by plant life.  There i
+s a large stone archway to the north acting as the doorway to the ruined complex.  A crevice
+ in the rock to the east leads to an alarmingly dark passageway.                            
+There are 2 exits:                                                                          
+- east                                                                                      
+- north                                                                                     </t>
+  </si>
+  <si>
+    <t>== Ruins == (2452)
+You are in the once-opulent foyer of a massive ruined complex.  There is a door to the south leading to the overgrowth outside and stairs to the north which lead into a larger hall.
+Things of interest here:
+- red coin
+There are 2 exits:
+- north
 - south</t>
   </si>
   <si>
-    <t>2387</t>
+    <t>== Ruins == (2457)
+You stand in the massive central hall of these ruins.  The walls are crumbling, and vegetation has clearly taken over.  Rooms are attached in all directions.  There is a strange monument in the center of the hall with circular slots and unusual symbols.  It reads:
+_ + _ * _^2 + _^3 - _ = 399
+There are 4 exits:
+- north
+- south
+- east
+- west</t>
+  </si>
+  <si>
+    <t>== Ruins == (2468)
+You stand in what seems to have once been a dining hall; broken tables and pottery are scattered everywhere.  A staircase here leads down.
+Things of interest here:
+- concave coin
+There are 2 exits:
+- down
+- west</t>
+  </si>
+  <si>
+    <t>== Ruins == (2478)
+You find yourself in what was once the living quarters for the complex.  Many smaller rooms which once had walls to divide them now lay in disarray.  There is a staircase up here.
+Things of interest here:
+- blue coin
+There are 2 exits:
+- up
+- east</t>
+  </si>
+  <si>
+    <t>Up from 2478
+== Ruins == (2483)
+This was long ago a lavish throne room.  Dried-up fountains and crumbling statues line the walls, and the carved stone throne in the center of the room is falling apart.
+Things of interest here:
+- shiny coin
+There is 1 exit:
+- down</t>
+  </si>
+  <si>
+    <t>Down from 2457
+== Ruins == (2473)
+This seems to be a kitchen; there are brick stoves and shelves along the wall.  Everything here has fallen into disrepair.
+Things of interest here:
+- corroded coin
+There is 1 exit:
+- up</t>
   </si>
 </sst>
 </file>
@@ -672,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393A6616-64D5-4724-A439-678ACFE4F18C}">
-  <dimension ref="A13:J22"/>
+  <dimension ref="B12:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,132 +791,179 @@
     <col min="1" max="16384" width="47.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G13" s="7"/>
-      <c r="H13" s="7" t="s">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="2:13" ht="225" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="165" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="H16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="C14" s="6" t="s">
+      <c r="K16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="300" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="G18" s="8"/>
+      <c r="H18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="H19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="I19" s="7"/>
+      <c r="J19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="L20" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="F21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="L21" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="D22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="4" t="s">
+      <c r="E22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="F22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="G22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="E16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="4:9" ht="300" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="4:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="D18" s="8"/>
-      <c r="E18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="4:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="E19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="4:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="I20" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="4:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="I21" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="I22" s="3" t="s">
+      <c r="L22" s="3" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on orb program
</commit_message>
<xml_diff>
--- a/synacor/rpg_maze.xlsx
+++ b/synacor/rpg_maze.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\AoC2019\synacor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4361C47F-9C70-4925-95BF-54ED26F5901B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1B430BC-D6C2-4419-BAF2-0EB768D8FA13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="795" windowWidth="21600" windowHeight="11385" xr2:uid="{A4590512-B461-4D61-BB7F-4AF2383C5086}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
   <si>
     <t>== Foothills ==
 You find yourself standing at the base of an enormous mountain.  At its base to the north, there is a massive doorway.  A sign nearby reads "Keep out!  Definitely no treasure within!"
@@ -581,6 +582,102 @@
   </si>
   <si>
     <t>30</t>
+  </si>
+  <si>
+    <t>== Beach == 2498
+This is a sandy beach in a cove on some tropical island.  It is raining.  The ocean is to your south, and heavy foliage is to your north; the beach extends west and east.
+There are 3 exits:
+- west
+- east
+- north</t>
+  </si>
+  <si>
+    <t>== Beach == 2503
+This is a sandy beach in a cove on some tropical island.  It is raining.  To your west is an embankment of the cove which looks too steep to climb.  The beach extends to the east, and there is dense foliage to the north.  The ocean to the south seems uninviting.
+There are 2 exits:
+- east
+- north</t>
+  </si>
+  <si>
+    <t>== Tropical Island == 2513
+The large trees here seem to be protecting you from the rain.  As you push through the undergrowth, you can hear birds chirping overhead.  There is a steep rock face to your west blocking your path.
+There are 3 exits:
+- north
+- south
+- east</t>
+  </si>
+  <si>
+    <t>== Tropical Island == 2523
+The embankment of the cove come toegher here to your east and west.  Between these tall rock faces, there is a narrow, overgrown path leading north.  You hear waves lapping up on a beach through the dense vegetation to your south.
+There are 2 exits:
+- north
+- south</t>
+  </si>
+  <si>
+    <t>== Tropical Island == 2528
+You are on a narrow path between two steep rock faces which look like they have been here for thousands of years.  Rain trickles down through the vegetation and moss, and through the leaves you can occasionally see a sliver of light hundreds of feet above you where the rock walls end.
+There are 2 exits:
+- north
+- south</t>
+  </si>
+  <si>
+    <t>== Tropical Island == 2533
+The narrow path slopes downward to the north and leads to the mouth of a small cave.  A sign nearby reads "Treasure Vault Access", but different handwriting has crossed this out and written "Lair of Horrible Monster!  All non-pirates keep out!".
+There are 2 exits:
+- north
+- south</t>
+  </si>
+  <si>
+    <t>== Tropical Cave == 2538
+You stand at the entrance to a natural cave which looks like it hasn't been visited in quite some time.  Light pours in through the opening to the south, while fireflies light the path further into the cave to the north.
+There are 2 exits:
+- north
+- south</t>
+  </si>
+  <si>
+    <t>== Tropical Cave == 2543
+Fireflies slowly drift around you and light the tunnel, which seems to get brighter to the south, but dimmer to the north.
+There are 2 exits:
+- north
+- south</t>
+  </si>
+  <si>
+    <t>== Tropical Cave == 2548
+The cave is a little wider here.  You find the cobweb-encrusted remains of a small camp, and although you don't suspect the broken pieces of tables and chairs will prove useful to your quest, the fireflies seem to like using the debris as a shelter.  A passageway leads north and south, and there is an alcove to the east.
+There are 3 exits:
+- north
+- south
+- east</t>
+  </si>
+  <si>
+    <t>== Tropical Cave Alcove == 2553
+At the back of this alcove, there is a small table, a chair, and a broken lantern.  It looks like this space was used much more recently than the camp to the west.
+Things of interest here:
+- journal
+There is 1 exit:
+- west</t>
+  </si>
+  <si>
+    <t>== Tropical Cave == 2558
+This tunnel slopes deeper underground to the north, but the fireflies are all around to light your path.
+There are 2 exits:
+- north
+- south</t>
+  </si>
+  <si>
+    <t>== Tropical Island == 2518
+The east embankment of the cove towers over you.  It produces a small waterfall here which cascades excitedly into a pool.
+There are 3 exits:
+- north
+- south
+- west</t>
+  </si>
+  <si>
+    <t>== Beach == 2508
+This is a sandy beach in a cove on some tropical island.  It is raining.  The steep cove embankment to your east blocks your path, and the ocean waters here look unsafe.  The beach extends to the west, and there is dense foliage to the north.
+There are 2 exits:
+- west
+- north</t>
   </si>
 </sst>
 </file>
@@ -1008,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393A6616-64D5-4724-A439-678ACFE4F18C}">
-  <dimension ref="B12:M60"/>
+  <dimension ref="B12:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B50" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="E35" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,17 +1293,118 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="3:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+    </row>
+    <row r="36" spans="3:13" ht="105" x14ac:dyDescent="0.25">
       <c r="C36" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="3:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+    </row>
+    <row r="37" spans="3:13" ht="210" x14ac:dyDescent="0.25">
       <c r="C37" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+    </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+    </row>
+    <row r="41" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+    </row>
+    <row r="42" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="I42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="F43" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+    </row>
+    <row r="45" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="F45" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="3:13" x14ac:dyDescent="0.25">
       <c r="F48" s="5" t="s">
         <v>52</v>
       </c>
@@ -1267,68 +1465,63 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="5"/>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="F56" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C58" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C59" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C60" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>65</v>
+    <row r="53" spans="3:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="C53" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" ht="195" x14ac:dyDescent="0.25">
+      <c r="C54" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="C55" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="C56" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="C57" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="C58" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="C59" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" s="4"/>
+    </row>
+    <row r="60" spans="3:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="C60" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="3:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="C61" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>